<commit_message>
Changes to practice programs package->Collections program
</commit_message>
<xml_diff>
--- a/SeleniumJava/Excel.xlsx
+++ b/SeleniumJava/Excel.xlsx
@@ -2,16 +2,17 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="11955" windowHeight="2280"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
-    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -34,7 +35,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -62,16 +62,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -80,10 +80,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -239,7 +239,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -248,13 +248,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -264,7 +264,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -273,7 +273,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -282,7 +282,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -292,12 +292,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -328,7 +328,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -347,7 +347,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -360,15 +360,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -379,7 +379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -390,7 +390,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -402,7 +402,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -414,7 +414,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -426,6 +426,6 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>